<commit_message>
imports almost finished, package missing
</commit_message>
<xml_diff>
--- a/travel_flight/data/Vuelos.xlsx
+++ b/travel_flight/data/Vuelos.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roly\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\openerp_travel\openerp_travel\travel_flight\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Vuelos" sheetId="1" r:id="rId1"/>
-    <sheet name="Precios" sheetId="2" r:id="rId2"/>
-    <sheet name="Proveedores" sheetId="3" r:id="rId3"/>
+    <sheet name="Proveedores" sheetId="3" r:id="rId2"/>
+    <sheet name="Precios" sheetId="2" r:id="rId3"/>
     <sheet name="Suplementos" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>Nombre</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Dirección</t>
   </si>
   <si>
-    <t>Sitio Web</t>
-  </si>
-  <si>
     <t>Teléfono</t>
   </si>
   <si>
@@ -59,9 +56,6 @@
     <t>Fax</t>
   </si>
   <si>
-    <t>Fecha incio</t>
-  </si>
-  <si>
     <t>Precio</t>
   </si>
   <si>
@@ -84,16 +78,27 @@
   </si>
   <si>
     <t>Niños</t>
+  </si>
+  <si>
+    <t>Sitio web</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -116,13 +121,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -437,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,10 +461,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -465,10 +474,59 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="D2" s="2"/>
+      <c r="F2" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="A2" sqref="A2:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,7 +539,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
@@ -493,10 +551,10 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -504,50 +562,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A2" sqref="A2:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,26 +581,29 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>11</v>
-      </c>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>